<commit_message>
Atualizando tabela e modelo conceitual (Endereços)
</commit_message>
<xml_diff>
--- a/arquivos/ComprasOnlineNormalizada.xlsx
+++ b/arquivos/ComprasOnlineNormalizada.xlsx
@@ -10,8 +10,8 @@
     <sheet state="visible" name="Endereco" sheetId="5" r:id="rId7"/>
     <sheet state="visible" name="Mensagens_administrador" sheetId="6" r:id="rId8"/>
     <sheet state="visible" name="Produto_Marca" sheetId="7" r:id="rId9"/>
-    <sheet state="visible" name="Produto_consumo_medio_cliente" sheetId="8" r:id="rId10"/>
-    <sheet state="visible" name="Supermercado" sheetId="9" r:id="rId11"/>
+    <sheet state="visible" name="Supermercado" sheetId="8" r:id="rId10"/>
+    <sheet state="visible" name="Produto_consumo_medio_cliente" sheetId="9" r:id="rId11"/>
     <sheet state="visible" name="Produto_consumo_medio_administr" sheetId="10" r:id="rId12"/>
     <sheet state="visible" name="Supermercado_preferencia_admini" sheetId="11" r:id="rId13"/>
   </sheets>
@@ -145,7 +145,7 @@
     <author/>
   </authors>
   <commentList>
-    <comment authorId="0" ref="A1">
+    <comment authorId="0" ref="B1">
       <text>
         <t xml:space="preserve">Está no modelo conceitual
 	-Leticia Teixeira</t>
@@ -193,6 +193,22 @@
     <author/>
   </authors>
   <commentList>
+    <comment authorId="0" ref="A1">
+      <text>
+        <t xml:space="preserve">Está incompleto no modelo conceitual
+	-Leticia Teixeira</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments9.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author/>
+  </authors>
+  <commentList>
     <comment authorId="0" ref="B2">
       <text>
         <t xml:space="preserve">O que pode ser o consumo médio?
@@ -209,44 +225,55 @@
 </comments>
 </file>
 
-<file path=xl/comments9.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <authors>
-    <author/>
-  </authors>
-  <commentList>
-    <comment authorId="0" ref="A1">
-      <text>
-        <t xml:space="preserve">Está incompleto no modelo conceitual
-	-Leticia Teixeira</t>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="127">
+  <si>
+    <t>PRODUTO_COMPRA</t>
+  </si>
   <si>
     <t>PRODUTO_ESTOQUE</t>
-  </si>
-  <si>
-    <t>PRODUTO_COMPRA</t>
   </si>
   <si>
     <t>USUARIO</t>
   </si>
   <si>
+    <t>codigo (integer)</t>
+  </si>
+  <si>
     <t>cod_produto_fk (integer) *</t>
   </si>
   <si>
-    <t>codigo (integer)</t>
+    <t>id (INTEGER)</t>
   </si>
   <si>
-    <t>id_usuario (INTEGER)</t>
+    <t>qnt_minima (integer)</t>
   </si>
   <si>
     <t>email (varchar(50))</t>
+  </si>
+  <si>
+    <t>nome (varchar(20))</t>
+  </si>
+  <si>
+    <t>qnt_atual (integer)</t>
+  </si>
+  <si>
+    <t>usuario_id_fk (int) *</t>
+  </si>
+  <si>
+    <t>sobrenome (varchar(20))</t>
+  </si>
+  <si>
+    <t>dat_nascimento (date)</t>
+  </si>
+  <si>
+    <t>endereco_id_fk (int) *</t>
+  </si>
+  <si>
+    <t>senha (varchar(20))</t>
+  </si>
+  <si>
+    <t>administrador (bool)</t>
   </si>
   <si>
     <t>qnt_compra (integer)</t>
@@ -258,34 +285,7 @@
     <t>preco (money)</t>
   </si>
   <si>
-    <t>usuario_id_fk (int) *</t>
-  </si>
-  <si>
     <t>data_compra (date)</t>
-  </si>
-  <si>
-    <t>qnt_minima (integer)</t>
-  </si>
-  <si>
-    <t>qnt_atual (integer)</t>
-  </si>
-  <si>
-    <t>nome (varchar(20))</t>
-  </si>
-  <si>
-    <t>sobrenome (varchar(20))</t>
-  </si>
-  <si>
-    <t>dat_nascimento (date)</t>
-  </si>
-  <si>
-    <t>endereco_cep_fk (int) *</t>
-  </si>
-  <si>
-    <t>senha (varchar(20))</t>
-  </si>
-  <si>
-    <t>administrador (bool)</t>
   </si>
   <si>
     <t>joao_silva@gmail.com</t>
@@ -295,9 +295,6 @@
   </si>
   <si>
     <t>Silva</t>
-  </si>
-  <si>
-    <t>29065-220</t>
   </si>
   <si>
     <t>goiaba33</t>
@@ -315,9 +312,6 @@
     <t>Pereira</t>
   </si>
   <si>
-    <t>29160-210</t>
-  </si>
-  <si>
     <t>xd12345</t>
   </si>
   <si>
@@ -328,9 +322,6 @@
   </si>
   <si>
     <t>Oliveira</t>
-  </si>
-  <si>
-    <t>29165-360</t>
   </si>
   <si>
     <t>zezin99</t>
@@ -345,9 +336,6 @@
     <t>Souza</t>
   </si>
   <si>
-    <t>29165-800</t>
-  </si>
-  <si>
     <t>arrow123</t>
   </si>
   <si>
@@ -360,19 +348,16 @@
     <t>Alderson</t>
   </si>
   <si>
-    <t>29101-441</t>
-  </si>
-  <si>
     <t>fsociety12</t>
   </si>
   <si>
     <t>verdadeiro</t>
   </si>
   <si>
-    <t xml:space="preserve"> .</t>
+    <t>PRODUTO_UNID</t>
   </si>
   <si>
-    <t>PRODUTO_UNID</t>
+    <t xml:space="preserve"> .</t>
   </si>
   <si>
     <t>marca_fk (integer) *</t>
@@ -384,19 +369,10 @@
     <t>quant (integer)</t>
   </si>
   <si>
-    <t>l</t>
+    <t>ENDERECO</t>
   </si>
   <si>
-    <t>g</t>
-  </si>
-  <si>
-    <t>kg</t>
-  </si>
-  <si>
-    <t>unid</t>
-  </si>
-  <si>
-    <t>ENDERECO</t>
+    <t>id (serial)</t>
   </si>
   <si>
     <t>cep (int)</t>
@@ -417,6 +393,18 @@
     <t>29165-491</t>
   </si>
   <si>
+    <t>l</t>
+  </si>
+  <si>
+    <t>g</t>
+  </si>
+  <si>
+    <t>kg</t>
+  </si>
+  <si>
+    <t>unid</t>
+  </si>
+  <si>
     <t xml:space="preserve">ES </t>
   </si>
   <si>
@@ -429,19 +417,58 @@
     <t>Rua Afonso Arinos Melo Franco</t>
   </si>
   <si>
+    <t>29165-360</t>
+  </si>
+  <si>
     <t>ES</t>
   </si>
   <si>
     <t>Rua Almirante Tamandaré</t>
   </si>
   <si>
-    <t>MENSAGENS_ADMINISTRADOR</t>
+    <t>29165-800</t>
   </si>
   <si>
     <t>Valparaíso</t>
   </si>
   <si>
     <t>Avenida Iriri</t>
+  </si>
+  <si>
+    <t>29060-210</t>
+  </si>
+  <si>
+    <t>Vitória</t>
+  </si>
+  <si>
+    <t>Jardim da Penha</t>
+  </si>
+  <si>
+    <t>Rua Adriano Fontana</t>
+  </si>
+  <si>
+    <t>29065-220</t>
+  </si>
+  <si>
+    <t>Mata da Praia</t>
+  </si>
+  <si>
+    <t>Rua Alderico Tristão</t>
+  </si>
+  <si>
+    <t>29101-441</t>
+  </si>
+  <si>
+    <t>Vila Velha</t>
+  </si>
+  <si>
+    <t>Praia da Costa</t>
+  </si>
+  <si>
+    <t>Avenida Afonso Pena</t>
+  </si>
+  <si>
+    <t>MENSAGENS_ADMINISTRADOR</t>
   </si>
   <si>
     <t>mensagem (text)</t>
@@ -462,7 +489,7 @@
     <t>[...]Texto 4[...]</t>
   </si>
   <si>
-    <t>29060-210</t>
+    <t>PRODUTO_MARCA</t>
   </si>
   <si>
     <t>[...]Texto 5[...]</t>
@@ -471,46 +498,19 @@
     <t>[...]Texto 6[...]</t>
   </si>
   <si>
-    <t>[...]Texto 7[...]</t>
+    <t>marca (varchar(20))</t>
   </si>
   <si>
-    <t>[...]Texto 8[...]</t>
-  </si>
-  <si>
-    <t>Vitória</t>
-  </si>
-  <si>
-    <t>Jardim da Penha</t>
-  </si>
-  <si>
-    <t>Rua Adriano Fontana</t>
-  </si>
-  <si>
-    <t>Mata da Praia</t>
-  </si>
-  <si>
-    <t>Rua Alderico Tristão</t>
-  </si>
-  <si>
-    <t>Vila Velha</t>
-  </si>
-  <si>
-    <t>Praia da Costa</t>
-  </si>
-  <si>
-    <t>Avenida Afonso Pena</t>
-  </si>
-  <si>
-    <t>PRODUTO_MARCA</t>
-  </si>
-  <si>
-    <t>marca (varchar(20))</t>
+    <t>[...]Texto 7[...]</t>
   </si>
   <si>
     <t xml:space="preserve">Sorvete </t>
   </si>
   <si>
     <t>Kibom</t>
+  </si>
+  <si>
+    <t>[...]Texto 8[...]</t>
   </si>
   <si>
     <t xml:space="preserve">Biscoito </t>
@@ -570,7 +570,13 @@
     <t>PRODUTO_CONSUMO_MEDIO_CLIENTE</t>
   </si>
   <si>
+    <t>SUPERMERCADO</t>
+  </si>
+  <si>
     <t>produto_fk (int)*</t>
+  </si>
+  <si>
+    <t>Perim</t>
   </si>
   <si>
     <t>cosumo_medio (float)</t>
@@ -583,12 +589,6 @@
   </si>
   <si>
     <t>usuario_fk *</t>
-  </si>
-  <si>
-    <t>SUPERMERCADO</t>
-  </si>
-  <si>
-    <t>Perim</t>
   </si>
   <si>
     <t>ExtraBom</t>
@@ -615,8 +615,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <numFmts count="4">
     <numFmt numFmtId="164" formatCode="[$R$ -416]#,##0.00"/>
-    <numFmt numFmtId="165" formatCode="dd/mm/yyyy"/>
-    <numFmt numFmtId="166" formatCode="DD/MM/YYYY"/>
+    <numFmt numFmtId="165" formatCode="DD/MM/YYYY"/>
+    <numFmt numFmtId="166" formatCode="dd/mm/yyyy"/>
     <numFmt numFmtId="167" formatCode="D/M/YYYY"/>
   </numFmts>
   <fonts count="9">
@@ -721,32 +721,32 @@
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="4" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="0" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
+    <xf borderId="0" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="166" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="5" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" vertical="center"/>
@@ -769,23 +769,23 @@
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="5" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="6" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
-    </xf>
     <xf borderId="0" fillId="4" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
+    <xf borderId="0" fillId="5" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="6" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
     <xf borderId="0" fillId="2" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" vertical="center"/>
@@ -799,17 +799,17 @@
     <xf borderId="0" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
+    <xf borderId="0" fillId="5" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="0" fillId="7" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="5" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
     <xf borderId="0" fillId="5" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="166" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -911,26 +911,26 @@
       <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="7" t="s">
-        <v>6</v>
+      <c r="B2" s="3" t="s">
+        <v>7</v>
       </c>
       <c r="C2" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="H2" s="5" t="s">
         <v>15</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="H2" s="5" t="s">
-        <v>19</v>
       </c>
       <c r="I2" s="2"/>
       <c r="O2" s="2"/>
@@ -939,29 +939,29 @@
       <c r="AB2" s="2"/>
     </row>
     <row r="3">
-      <c r="A3" s="6">
+      <c r="A3" s="7">
         <v>1.0</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="D3" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="E3" s="11">
+      <c r="E3" s="10">
         <v>35197.0</v>
       </c>
-      <c r="F3" s="12" t="s">
+      <c r="F3" s="12">
+        <v>4.0</v>
+      </c>
+      <c r="G3" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="G3" s="13" t="s">
+      <c r="H3" s="7" t="s">
         <v>24</v>
-      </c>
-      <c r="H3" s="6" t="s">
-        <v>25</v>
       </c>
       <c r="I3" s="2"/>
       <c r="O3" s="2"/>
@@ -970,29 +970,29 @@
       <c r="AB3" s="2"/>
     </row>
     <row r="4">
-      <c r="A4" s="6">
+      <c r="A4" s="7">
         <v>2.0</v>
       </c>
       <c r="B4" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="D4" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="E4" s="10">
+        <v>33056.0</v>
+      </c>
+      <c r="F4" s="14">
+        <v>3.0</v>
+      </c>
+      <c r="G4" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E4" s="11">
-        <v>33056.0</v>
-      </c>
-      <c r="F4" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="H4" s="6" t="s">
-        <v>25</v>
+      <c r="H4" s="7" t="s">
+        <v>24</v>
       </c>
       <c r="I4" s="2"/>
       <c r="O4" s="2"/>
@@ -1001,29 +1001,29 @@
       <c r="AB4" s="2"/>
     </row>
     <row r="5">
-      <c r="A5" s="6">
+      <c r="A5" s="7">
         <v>3.0</v>
       </c>
       <c r="B5" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="E5" s="10">
+        <v>36412.0</v>
+      </c>
+      <c r="F5" s="14">
+        <v>1.0</v>
+      </c>
+      <c r="G5" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="E5" s="11">
-        <v>36412.0</v>
-      </c>
-      <c r="F5" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="H5" s="6" t="s">
-        <v>25</v>
+      <c r="H5" s="7" t="s">
+        <v>24</v>
       </c>
       <c r="I5" s="2"/>
       <c r="O5" s="2"/>
@@ -1032,29 +1032,29 @@
       <c r="AB5" s="2"/>
     </row>
     <row r="6">
-      <c r="A6" s="6">
+      <c r="A6" s="7">
         <v>4.0</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="E6" s="15">
         <v>36883.0</v>
       </c>
-      <c r="F6" s="14" t="s">
-        <v>39</v>
+      <c r="F6" s="14">
+        <v>2.0</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="H6" s="6" t="s">
-        <v>25</v>
+        <v>36</v>
+      </c>
+      <c r="H6" s="7" t="s">
+        <v>24</v>
       </c>
       <c r="I6" s="2"/>
       <c r="O6" s="2"/>
@@ -1069,29 +1069,29 @@
       <c r="AB6" s="2"/>
     </row>
     <row r="7">
-      <c r="A7" s="6">
+      <c r="A7" s="7">
         <v>5.0</v>
       </c>
       <c r="B7" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E7" s="10">
+        <v>29718.0</v>
+      </c>
+      <c r="F7" s="14">
+        <v>5.0</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="H7" s="7" t="s">
         <v>41</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="E7" s="11">
-        <v>29718.0</v>
-      </c>
-      <c r="F7" s="14" t="s">
-        <v>44</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="H7" s="6" t="s">
-        <v>46</v>
       </c>
       <c r="I7" s="2"/>
       <c r="O7" s="2"/>
@@ -1387,11 +1387,11 @@
       <c r="AB18" s="2"/>
     </row>
     <row r="19">
-      <c r="A19" s="6"/>
+      <c r="A19" s="7"/>
       <c r="H19" s="16"/>
       <c r="L19" s="2"/>
-      <c r="M19" s="6"/>
-      <c r="N19" s="6"/>
+      <c r="M19" s="7"/>
+      <c r="N19" s="7"/>
       <c r="O19" s="2"/>
       <c r="P19" s="2"/>
       <c r="Q19" s="2"/>
@@ -1430,8 +1430,8 @@
     </row>
     <row r="21">
       <c r="A21" s="18"/>
-      <c r="H21" s="6" t="s">
-        <v>47</v>
+      <c r="H21" s="7" t="s">
+        <v>43</v>
       </c>
       <c r="L21" s="12"/>
       <c r="M21" s="2"/>
@@ -1473,7 +1473,7 @@
       <c r="AB22" s="2"/>
     </row>
     <row r="23">
-      <c r="A23" s="19"/>
+      <c r="A23" s="21"/>
       <c r="H23" s="2"/>
       <c r="I23" s="2"/>
       <c r="J23" s="2"/>
@@ -1497,7 +1497,7 @@
       <c r="AB23" s="2"/>
     </row>
     <row r="24">
-      <c r="A24" s="19"/>
+      <c r="A24" s="21"/>
       <c r="H24" s="2"/>
       <c r="I24" s="2"/>
       <c r="J24" s="2"/>
@@ -1545,7 +1545,7 @@
       <c r="AB25" s="2"/>
     </row>
     <row r="26">
-      <c r="A26" s="19"/>
+      <c r="A26" s="21"/>
       <c r="H26" s="2"/>
       <c r="I26" s="2"/>
       <c r="J26" s="2"/>
@@ -1636,7 +1636,7 @@
       <c r="E29" s="2"/>
       <c r="F29" s="2"/>
       <c r="G29" s="2"/>
-      <c r="H29" s="20"/>
+      <c r="H29" s="24"/>
       <c r="I29" s="2"/>
       <c r="J29" s="2"/>
       <c r="K29" s="2"/>
@@ -30818,87 +30818,87 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="29" t="s">
+      <c r="A2" s="30" t="s">
         <v>123</v>
       </c>
-      <c r="B2" s="29" t="s">
-        <v>115</v>
-      </c>
-      <c r="C2" s="29" t="s">
-        <v>116</v>
-      </c>
-      <c r="D2" s="29" t="s">
+      <c r="B2" s="30" t="s">
         <v>117</v>
       </c>
-      <c r="E2" s="29" t="s">
+      <c r="C2" s="30" t="s">
         <v>118</v>
       </c>
+      <c r="D2" s="30" t="s">
+        <v>119</v>
+      </c>
+      <c r="E2" s="30" t="s">
+        <v>120</v>
+      </c>
     </row>
     <row r="3">
-      <c r="A3" s="24">
+      <c r="A3" s="23">
         <v>1.0</v>
       </c>
-      <c r="B3" s="24">
+      <c r="B3" s="23">
         <v>7.0</v>
       </c>
-      <c r="C3" s="30">
+      <c r="C3" s="32">
         <v>43525.0</v>
       </c>
-      <c r="D3" s="30">
+      <c r="D3" s="32">
         <v>43555.0</v>
       </c>
-      <c r="E3" s="24">
+      <c r="E3" s="23">
         <v>1.0</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="24">
+      <c r="A4" s="23">
         <v>5.0</v>
       </c>
-      <c r="B4" s="24">
+      <c r="B4" s="23">
         <v>8.0</v>
       </c>
-      <c r="C4" s="30">
+      <c r="C4" s="32">
         <v>43497.0</v>
       </c>
-      <c r="D4" s="30">
+      <c r="D4" s="32">
         <v>43524.0</v>
       </c>
-      <c r="E4" s="24">
+      <c r="E4" s="23">
         <v>2.0</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="24">
+      <c r="A5" s="23">
         <v>4.0</v>
       </c>
-      <c r="B5" s="24">
+      <c r="B5" s="23">
         <v>4.0</v>
       </c>
-      <c r="C5" s="30">
+      <c r="C5" s="32">
         <v>43556.0</v>
       </c>
-      <c r="D5" s="30">
+      <c r="D5" s="32">
         <v>43585.0</v>
       </c>
-      <c r="E5" s="24">
+      <c r="E5" s="23">
         <v>4.0</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="24">
+      <c r="A6" s="23">
         <v>9.0</v>
       </c>
-      <c r="B6" s="24">
+      <c r="B6" s="23">
         <v>6.0</v>
       </c>
-      <c r="C6" s="30">
+      <c r="C6" s="32">
         <v>43586.0</v>
       </c>
-      <c r="D6" s="30">
+      <c r="D6" s="32">
         <v>43616.0</v>
       </c>
-      <c r="E6" s="24">
+      <c r="E6" s="23">
         <v>5.0</v>
       </c>
     </row>
@@ -30933,44 +30933,44 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="29" t="s">
+      <c r="A2" s="30" t="s">
         <v>125</v>
       </c>
-      <c r="B2" s="29" t="s">
+      <c r="B2" s="30" t="s">
         <v>126</v>
       </c>
-      <c r="C2" s="29" t="s">
-        <v>116</v>
-      </c>
-      <c r="D2" s="29" t="s">
-        <v>117</v>
+      <c r="C2" s="30" t="s">
+        <v>118</v>
+      </c>
+      <c r="D2" s="30" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="24">
+      <c r="A3" s="23">
         <v>1.0</v>
       </c>
-      <c r="B3" s="24">
+      <c r="B3" s="23">
         <v>10.0</v>
       </c>
-      <c r="C3" s="30">
+      <c r="C3" s="32">
         <v>43525.0</v>
       </c>
-      <c r="D3" s="30">
+      <c r="D3" s="32">
         <v>43555.0</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="24">
+      <c r="A4" s="23">
         <v>2.0</v>
       </c>
-      <c r="B4" s="24">
+      <c r="B4" s="23">
         <v>12.0</v>
       </c>
-      <c r="C4" s="30">
+      <c r="C4" s="32">
         <v>43556.0</v>
       </c>
-      <c r="D4" s="30">
+      <c r="D4" s="32">
         <v>43585.0</v>
       </c>
     </row>
@@ -31001,90 +31001,90 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="7" t="s">
-        <v>3</v>
+      <c r="A2" s="3" t="s">
+        <v>4</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="6">
+      <c r="A3" s="7">
         <v>1.0</v>
       </c>
-      <c r="B3" s="6">
+      <c r="B3" s="7">
         <v>1.0</v>
       </c>
-      <c r="C3" s="6">
+      <c r="C3" s="7">
         <v>0.0</v>
       </c>
-      <c r="D3" s="6">
+      <c r="D3" s="7">
         <v>1.0</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="6">
+      <c r="A4" s="7">
         <v>3.0</v>
       </c>
-      <c r="B4" s="6">
+      <c r="B4" s="7">
         <v>3.0</v>
       </c>
-      <c r="C4" s="6">
+      <c r="C4" s="7">
         <v>2.0</v>
       </c>
-      <c r="D4" s="6">
+      <c r="D4" s="7">
         <v>2.0</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="6">
+      <c r="A5" s="7">
         <v>6.0</v>
       </c>
-      <c r="B5" s="6">
+      <c r="B5" s="7">
         <v>1.0</v>
       </c>
-      <c r="C5" s="6">
+      <c r="C5" s="7">
         <v>1.0</v>
       </c>
-      <c r="D5" s="6">
+      <c r="D5" s="7">
         <v>3.0</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="6">
+      <c r="A6" s="7">
         <v>9.0</v>
       </c>
-      <c r="B6" s="6">
+      <c r="B6" s="7">
         <v>2.0</v>
       </c>
-      <c r="C6" s="6">
+      <c r="C6" s="7">
         <v>2.0</v>
       </c>
-      <c r="D6" s="6">
+      <c r="D6" s="7">
         <v>4.0</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="6">
+      <c r="A7" s="7">
         <v>8.0</v>
       </c>
-      <c r="B7" s="6">
+      <c r="B7" s="7">
         <v>1.0</v>
       </c>
-      <c r="C7" s="6">
+      <c r="C7" s="7">
         <v>0.0</v>
       </c>
-      <c r="D7" s="6">
+      <c r="D7" s="7">
         <v>2.0</v>
       </c>
     </row>
@@ -31117,98 +31117,98 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>3</v>
-      </c>
       <c r="C2" s="5" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="F2" s="5" t="s">
         <v>10</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="6">
+      <c r="A3" s="7">
         <v>1.0</v>
       </c>
-      <c r="B3" s="6">
+      <c r="B3" s="7">
         <v>1.0</v>
       </c>
-      <c r="C3" s="6">
+      <c r="C3" s="7">
         <v>1.0</v>
       </c>
-      <c r="D3" s="6">
+      <c r="D3" s="7">
         <v>2.0</v>
       </c>
-      <c r="E3" s="8">
+      <c r="E3" s="9">
         <v>14.99</v>
       </c>
-      <c r="F3" s="6">
+      <c r="F3" s="7">
         <v>1.0</v>
       </c>
-      <c r="G3" s="9">
+      <c r="G3" s="11">
         <v>43606.0</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="6">
+      <c r="A4" s="7">
         <v>2.0</v>
       </c>
-      <c r="B4" s="6">
+      <c r="B4" s="7">
         <v>3.0</v>
       </c>
-      <c r="C4" s="6">
+      <c r="C4" s="7">
         <v>1.0</v>
       </c>
-      <c r="D4" s="6">
+      <c r="D4" s="7">
         <v>1.0</v>
       </c>
-      <c r="E4" s="8">
+      <c r="E4" s="9">
         <v>8.49</v>
       </c>
-      <c r="F4" s="6">
+      <c r="F4" s="7">
         <v>2.0</v>
       </c>
-      <c r="G4" s="9">
+      <c r="G4" s="11">
         <v>43668.0</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="6">
+      <c r="A5" s="7">
         <v>3.0</v>
       </c>
-      <c r="B5" s="6">
+      <c r="B5" s="7">
         <v>8.0</v>
       </c>
-      <c r="C5" s="6">
+      <c r="C5" s="7">
         <v>1.0</v>
       </c>
-      <c r="D5" s="6">
+      <c r="D5" s="7">
         <v>1.0</v>
       </c>
-      <c r="E5" s="8">
+      <c r="E5" s="9">
         <v>17.99</v>
       </c>
-      <c r="F5" s="6">
+      <c r="F5" s="7">
         <v>2.0</v>
       </c>
-      <c r="G5" s="9">
+      <c r="G5" s="11">
         <v>43731.0</v>
       </c>
     </row>
@@ -31238,160 +31238,160 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="21" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="22" t="s">
-        <v>49</v>
+      <c r="A2" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="20" t="s">
+        <v>44</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="23">
+      <c r="A3" s="22">
         <v>1.0</v>
       </c>
-      <c r="B3" s="24">
+      <c r="B3" s="23">
         <v>1.0</v>
       </c>
-      <c r="C3" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="D3" s="6">
+      <c r="C3" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="D3" s="7">
         <v>2.0</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="23">
+      <c r="A4" s="22">
         <v>2.0</v>
       </c>
-      <c r="B4" s="24">
+      <c r="B4" s="23">
         <v>2.0</v>
       </c>
-      <c r="C4" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="D4" s="6">
+      <c r="C4" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="D4" s="7">
         <v>100.0</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="23">
+      <c r="A5" s="22">
         <v>3.0</v>
       </c>
-      <c r="B5" s="24">
+      <c r="B5" s="23">
         <v>3.0</v>
       </c>
-      <c r="C5" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="D5" s="6">
+      <c r="C5" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="D5" s="7">
         <v>100.0</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="23">
+      <c r="A6" s="22">
         <v>4.0</v>
       </c>
-      <c r="B6" s="24">
+      <c r="B6" s="23">
         <v>4.0</v>
       </c>
-      <c r="C6" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="D6" s="6">
+      <c r="C6" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="D6" s="7">
         <v>1.0</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="23">
+      <c r="A7" s="22">
         <v>5.0</v>
       </c>
-      <c r="B7" s="24">
+      <c r="B7" s="23">
         <v>5.0</v>
       </c>
-      <c r="C7" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="D7" s="6">
+      <c r="C7" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="D7" s="7">
         <v>500.0</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="23">
+      <c r="A8" s="22">
         <v>6.0</v>
       </c>
-      <c r="B8" s="24">
+      <c r="B8" s="23">
         <v>6.0</v>
       </c>
-      <c r="C8" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="D8" s="6">
+      <c r="C8" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="D8" s="7">
         <v>1.0</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="23">
+      <c r="A9" s="22">
         <v>7.0</v>
       </c>
-      <c r="B9" s="24">
+      <c r="B9" s="23">
         <v>7.0</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="C9" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="D9" s="7">
+        <v>6.0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="22">
+        <v>8.0</v>
+      </c>
+      <c r="B10" s="23">
+        <v>8.0</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="D10" s="7">
+        <v>5.0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="22">
+        <v>9.0</v>
+      </c>
+      <c r="B11" s="23">
+        <v>9.0</v>
+      </c>
+      <c r="C11" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="D9" s="6">
-        <v>6.0</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="23">
-        <v>8.0</v>
-      </c>
-      <c r="B10" s="24">
-        <v>8.0</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="D10" s="6">
-        <v>5.0</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="23">
-        <v>9.0</v>
-      </c>
-      <c r="B11" s="24">
-        <v>9.0</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="D11" s="6">
+      <c r="D11" s="7">
         <v>2.0</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="23">
+      <c r="A12" s="22">
         <v>10.0</v>
       </c>
-      <c r="B12" s="24">
+      <c r="B12" s="23">
         <v>10.0</v>
       </c>
-      <c r="C12" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="D12" s="6">
+      <c r="C12" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="D12" s="7">
         <v>3.0</v>
       </c>
     </row>
@@ -31414,158 +31414,179 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="3" max="3" width="15.43"/>
-    <col customWidth="1" min="4" max="4" width="17.86"/>
-    <col customWidth="1" min="5" max="5" width="27.0"/>
-    <col customWidth="1" min="6" max="6" width="27.43"/>
+    <col customWidth="1" min="4" max="4" width="15.43"/>
+    <col customWidth="1" min="5" max="5" width="17.86"/>
+    <col customWidth="1" min="6" max="6" width="27.0"/>
+    <col customWidth="1" min="7" max="7" width="27.43"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>58</v>
+        <v>48</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>49</v>
       </c>
       <c r="D2" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="12">
+        <v>0.0</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="D3" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E3" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F3" s="21" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="12" t="s">
+      <c r="G3" s="16" t="s">
         <v>62</v>
       </c>
-      <c r="C3" s="6" t="s">
+    </row>
+    <row r="4">
+      <c r="A4" s="12">
+        <v>1.0</v>
+      </c>
+      <c r="B4" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D4" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="E3" s="19" t="s">
+      <c r="E4" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="F4" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="G4" s="16" t="s">
         <v>65</v>
       </c>
-      <c r="F3" s="16" t="s">
+    </row>
+    <row r="5">
+      <c r="A5" s="12">
+        <v>2.0</v>
+      </c>
+      <c r="B5" s="21" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="C4" s="6" t="s">
+      <c r="D5" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="F5" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="G5" s="21" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="12">
+        <v>3.0</v>
+      </c>
+      <c r="B6" s="21" t="s">
+        <v>69</v>
+      </c>
+      <c r="D6" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="E4" s="19" t="s">
-        <v>65</v>
-      </c>
-      <c r="F4" s="16" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="19" t="s">
-        <v>39</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="D5" s="6" t="s">
+      <c r="E6" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="F6" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="G6" s="21" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="12">
+        <v>4.0</v>
+      </c>
+      <c r="B7" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="D7" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="E5" s="16" t="s">
+      <c r="E7" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="F5" s="19" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="19" t="s">
+      <c r="F7" s="16" t="s">
+        <v>74</v>
+      </c>
+      <c r="G7" s="16" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="12">
+        <v>5.0</v>
+      </c>
+      <c r="B8" s="21" t="s">
+        <v>76</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="F8" s="16" t="s">
         <v>78</v>
       </c>
-      <c r="C6" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="E6" s="16" t="s">
-        <v>84</v>
-      </c>
-      <c r="F6" s="19" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="E7" s="16" t="s">
-        <v>86</v>
-      </c>
-      <c r="F7" s="16" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="19" t="s">
-        <v>44</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="E8" s="16" t="s">
-        <v>89</v>
-      </c>
-      <c r="F8" s="19" t="s">
-        <v>90</v>
+      <c r="G8" s="21" t="s">
+        <v>79</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="8">
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="A1:G1"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink r:id="rId2" ref="A3"/>
-    <hyperlink r:id="rId3" ref="E3"/>
-    <hyperlink r:id="rId4" ref="A4"/>
-    <hyperlink r:id="rId5" ref="E4"/>
-    <hyperlink r:id="rId6" ref="A5"/>
-    <hyperlink r:id="rId7" ref="F5"/>
-    <hyperlink r:id="rId8" ref="A6"/>
-    <hyperlink r:id="rId9" ref="F6"/>
-    <hyperlink r:id="rId10" ref="A8"/>
-    <hyperlink r:id="rId11" ref="F8"/>
+    <hyperlink r:id="rId2" ref="B3"/>
+    <hyperlink r:id="rId3" ref="F3"/>
+    <hyperlink r:id="rId4" ref="B4"/>
+    <hyperlink r:id="rId5" ref="F4"/>
+    <hyperlink r:id="rId6" ref="B5"/>
+    <hyperlink r:id="rId7" ref="G5"/>
+    <hyperlink r:id="rId8" ref="B6"/>
+    <hyperlink r:id="rId9" ref="G6"/>
+    <hyperlink r:id="rId10" ref="B8"/>
+    <hyperlink r:id="rId11" ref="G8"/>
   </hyperlinks>
   <drawing r:id="rId12"/>
   <legacyDrawing r:id="rId13"/>
@@ -31589,105 +31610,105 @@
   <sheetData>
     <row r="1" ht="20.25" customHeight="1">
       <c r="A1" s="25" t="s">
-        <v>69</v>
+        <v>80</v>
       </c>
     </row>
     <row r="2" ht="27.75" customHeight="1">
       <c r="A2" s="26" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B2" s="27" t="s">
-        <v>72</v>
+        <v>81</v>
       </c>
       <c r="C2" s="27" t="s">
-        <v>73</v>
+        <v>82</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="24">
+      <c r="A3" s="23">
         <v>1.0</v>
       </c>
-      <c r="B3" s="24" t="s">
-        <v>74</v>
-      </c>
-      <c r="C3" s="24">
+      <c r="B3" s="23" t="s">
+        <v>83</v>
+      </c>
+      <c r="C3" s="23">
         <v>1.0</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="24">
+      <c r="A4" s="23">
         <v>2.0</v>
       </c>
-      <c r="B4" s="24" t="s">
-        <v>75</v>
-      </c>
-      <c r="C4" s="24">
+      <c r="B4" s="23" t="s">
+        <v>84</v>
+      </c>
+      <c r="C4" s="23">
         <v>2.0</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="24">
+      <c r="A5" s="23">
         <v>3.0</v>
       </c>
-      <c r="B5" s="24" t="s">
-        <v>76</v>
-      </c>
-      <c r="C5" s="24">
+      <c r="B5" s="23" t="s">
+        <v>85</v>
+      </c>
+      <c r="C5" s="23">
         <v>2.0</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="24">
+      <c r="A6" s="23">
         <v>4.0</v>
       </c>
-      <c r="B6" s="24" t="s">
-        <v>77</v>
-      </c>
-      <c r="C6" s="24">
+      <c r="B6" s="23" t="s">
+        <v>86</v>
+      </c>
+      <c r="C6" s="23">
         <v>5.0</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="24">
+      <c r="A7" s="23">
         <v>5.0</v>
       </c>
-      <c r="B7" s="24" t="s">
-        <v>79</v>
-      </c>
-      <c r="C7" s="24">
+      <c r="B7" s="23" t="s">
+        <v>88</v>
+      </c>
+      <c r="C7" s="23">
         <v>3.0</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="24">
+      <c r="A8" s="23">
         <v>6.0</v>
       </c>
-      <c r="B8" s="24" t="s">
-        <v>80</v>
-      </c>
-      <c r="C8" s="24">
+      <c r="B8" s="23" t="s">
+        <v>89</v>
+      </c>
+      <c r="C8" s="23">
         <v>4.0</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="24">
+      <c r="A9" s="23">
         <v>7.0</v>
       </c>
-      <c r="B9" s="24" t="s">
-        <v>81</v>
-      </c>
-      <c r="C9" s="24">
+      <c r="B9" s="23" t="s">
+        <v>91</v>
+      </c>
+      <c r="C9" s="23">
         <v>1.0</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="24">
+      <c r="A10" s="23">
         <v>8.0</v>
       </c>
-      <c r="B10" s="24" t="s">
-        <v>82</v>
-      </c>
-      <c r="C10" s="24">
+      <c r="B10" s="23" t="s">
+        <v>94</v>
+      </c>
+      <c r="C10" s="23">
         <v>2.0</v>
       </c>
     </row>
@@ -31717,129 +31738,129 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
+        <v>87</v>
+      </c>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
     </row>
     <row r="2">
       <c r="A2" s="4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="C2" s="5" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="7">
+        <v>1.0</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="6">
-        <v>1.0</v>
-      </c>
-      <c r="B3" s="2" t="s">
+      <c r="C3" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="C3" s="6" t="s">
-        <v>94</v>
-      </c>
     </row>
     <row r="4">
-      <c r="A4" s="6">
+      <c r="A4" s="7">
         <v>2.0</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="7" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="6">
+      <c r="A5" s="7">
         <v>3.0</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="7" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="6">
+      <c r="A6" s="7">
         <v>4.0</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="7" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="6">
+      <c r="A7" s="7">
         <v>5.0</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="7" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="6">
+      <c r="A8" s="7">
         <v>6.0</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="7" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="6">
+      <c r="A9" s="7">
         <v>7.0</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="C9" s="7" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="6">
+      <c r="A10" s="7">
         <v>8.0</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C10" s="7" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="6">
+      <c r="A11" s="7">
         <v>9.0</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="B11" s="7" t="s">
         <v>109</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C11" s="7" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="6">
+      <c r="A12" s="7">
         <v>10.0</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="B12" s="7" t="s">
         <v>111</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="C12" s="7" t="s">
         <v>112</v>
       </c>
     </row>
@@ -31862,105 +31883,54 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="16.57"/>
-    <col customWidth="1" min="2" max="2" width="22.0"/>
-    <col customWidth="1" min="3" max="3" width="21.0"/>
-    <col customWidth="1" min="4" max="4" width="19.57"/>
+    <col customWidth="1" min="2" max="2" width="17.0"/>
+    <col customWidth="1" min="3" max="3" width="24.0"/>
+    <col customWidth="1" min="4" max="4" width="15.57"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="28" t="s">
-        <v>113</v>
-      </c>
+      <c r="A1" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="D1" s="16"/>
     </row>
     <row r="2">
-      <c r="A2" s="29" t="s">
-        <v>114</v>
-      </c>
-      <c r="B2" s="29" t="s">
-        <v>115</v>
-      </c>
-      <c r="C2" s="29" t="s">
+      <c r="A2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="29"/>
+    </row>
+    <row r="3">
+      <c r="A3" s="7">
+        <v>0.0</v>
+      </c>
+      <c r="B3" s="7" t="s">
         <v>116</v>
       </c>
-      <c r="D2" s="29" t="s">
-        <v>117</v>
-      </c>
-      <c r="E2" s="29" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="24">
+      <c r="C3" s="31">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="7">
         <v>1.0</v>
       </c>
-      <c r="B3" s="24">
-        <v>7.0</v>
-      </c>
-      <c r="C3" s="30">
-        <v>43525.0</v>
-      </c>
-      <c r="D3" s="30">
-        <v>43555.0</v>
-      </c>
-      <c r="E3" s="24">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="24">
-        <v>5.0</v>
-      </c>
-      <c r="B4" s="24">
-        <v>8.0</v>
-      </c>
-      <c r="C4" s="30">
-        <v>43497.0</v>
-      </c>
-      <c r="D4" s="30">
-        <v>43524.0</v>
-      </c>
-      <c r="E4" s="24">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="24">
-        <v>4.0</v>
-      </c>
-      <c r="B5" s="24">
-        <v>4.0</v>
-      </c>
-      <c r="C5" s="30">
-        <v>43556.0</v>
-      </c>
-      <c r="D5" s="30">
-        <v>43585.0</v>
-      </c>
-      <c r="E5" s="24">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="24">
-        <v>9.0</v>
-      </c>
-      <c r="B6" s="24">
-        <v>6.0</v>
-      </c>
-      <c r="C6" s="30">
-        <v>43586.0</v>
-      </c>
-      <c r="D6" s="30">
-        <v>43616.0</v>
-      </c>
-      <c r="E6" s="24">
-        <v>5.0</v>
+      <c r="B4" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="C4" s="12">
+        <v>0.0</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A1:C1"/>
   </mergeCells>
   <drawing r:id="rId2"/>
   <legacyDrawing r:id="rId3"/>
@@ -31977,54 +31947,105 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="2" max="2" width="17.0"/>
-    <col customWidth="1" min="3" max="3" width="24.0"/>
-    <col customWidth="1" min="4" max="4" width="15.57"/>
+    <col customWidth="1" min="1" max="1" width="16.57"/>
+    <col customWidth="1" min="2" max="2" width="22.0"/>
+    <col customWidth="1" min="3" max="3" width="21.0"/>
+    <col customWidth="1" min="4" max="4" width="19.57"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="28" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="30" t="s">
+        <v>115</v>
+      </c>
+      <c r="B2" s="30" t="s">
+        <v>117</v>
+      </c>
+      <c r="C2" s="30" t="s">
+        <v>118</v>
+      </c>
+      <c r="D2" s="30" t="s">
         <v>119</v>
       </c>
-      <c r="D1" s="16"/>
-    </row>
-    <row r="2">
-      <c r="A2" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D2" s="31"/>
+      <c r="E2" s="30" t="s">
+        <v>120</v>
+      </c>
     </row>
     <row r="3">
-      <c r="A3" s="6">
+      <c r="A3" s="23">
         <v>1.0</v>
       </c>
-      <c r="B3" s="6" t="s">
-        <v>120</v>
-      </c>
-      <c r="C3" s="32" t="s">
-        <v>23</v>
+      <c r="B3" s="23">
+        <v>7.0</v>
+      </c>
+      <c r="C3" s="32">
+        <v>43525.0</v>
+      </c>
+      <c r="D3" s="32">
+        <v>43555.0</v>
+      </c>
+      <c r="E3" s="23">
+        <v>1.0</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="6">
+      <c r="A4" s="23">
+        <v>5.0</v>
+      </c>
+      <c r="B4" s="23">
+        <v>8.0</v>
+      </c>
+      <c r="C4" s="32">
+        <v>43497.0</v>
+      </c>
+      <c r="D4" s="32">
+        <v>43524.0</v>
+      </c>
+      <c r="E4" s="23">
         <v>2.0</v>
       </c>
-      <c r="B4" s="6" t="s">
-        <v>121</v>
-      </c>
-      <c r="C4" s="12" t="s">
-        <v>62</v>
+    </row>
+    <row r="5">
+      <c r="A5" s="23">
+        <v>4.0</v>
+      </c>
+      <c r="B5" s="23">
+        <v>4.0</v>
+      </c>
+      <c r="C5" s="32">
+        <v>43556.0</v>
+      </c>
+      <c r="D5" s="32">
+        <v>43585.0</v>
+      </c>
+      <c r="E5" s="23">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="23">
+        <v>9.0</v>
+      </c>
+      <c r="B6" s="23">
+        <v>6.0</v>
+      </c>
+      <c r="C6" s="32">
+        <v>43586.0</v>
+      </c>
+      <c r="D6" s="32">
+        <v>43616.0</v>
+      </c>
+      <c r="E6" s="23">
+        <v>5.0</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A1:E1"/>
   </mergeCells>
   <drawing r:id="rId2"/>
   <legacyDrawing r:id="rId3"/>

</xml_diff>